<commit_message>
Actualización de Diagrama ER y Normalización de tablas
Se agregó al diagrama las entidades de usuario, contacto usuario y bitacora. Y en el archivo de normalización de tablas se elimió variables sobrantes en usuario y contacto usuario.
</commit_message>
<xml_diff>
--- a/Normalizacion de tablas.xlsx
+++ b/Normalizacion de tablas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="60">
   <si>
     <t>1-tabla matricula_carrera, quizas se pueda saber el año de ingreso a travez de la matricula</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>1era forma normal</t>
+  </si>
+  <si>
+    <t>DETALLE</t>
   </si>
 </sst>
 </file>
@@ -346,7 +349,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -357,14 +359,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -375,9 +374,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,7 +689,7 @@
   <dimension ref="A2:P25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,66 +707,66 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:16" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="L3" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="27" t="s">
+      <c r="M3" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="N3" s="27" t="s">
+      <c r="N3" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="27" t="s">
+      <c r="O3" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="P3" s="27" t="s">
+      <c r="P3" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
+      <c r="A4" s="25"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
+      <c r="A5" s="25"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
+      <c r="A6" s="25"/>
     </row>
     <row r="8" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19" t="s">
         <v>44</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -777,33 +780,31 @@
       <c r="J8" s="21"/>
     </row>
     <row r="9" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="15">
         <v>1</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="16" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>40</v>
-      </c>
+      <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
       <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="9">
         <v>2</v>
       </c>
@@ -817,21 +818,19 @@
         <v>5</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="11" t="s">
         <v>24</v>
       </c>
+      <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="9">
         <v>3</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>37</v>
       </c>
       <c r="D11" s="11" t="s">
@@ -857,11 +856,11 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="9">
         <v>4</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="11" t="s">
@@ -879,11 +878,11 @@
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="25"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="9">
         <v>5</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="16" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="11" t="s">
@@ -901,11 +900,11 @@
       <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="9">
         <v>6</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="11" t="s">
@@ -923,11 +922,11 @@
       <c r="J14" s="12"/>
     </row>
     <row r="15" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="9">
         <v>7</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="11" t="s">
@@ -943,11 +942,11 @@
       <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="25"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="9">
         <v>8</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D16" s="11" t="s">
@@ -965,11 +964,11 @@
       <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="25"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="9">
         <v>9</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="11" t="s">
@@ -987,11 +986,11 @@
       <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="25"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="9">
         <v>10</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="11" t="s">
@@ -1009,11 +1008,11 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="25"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="9">
         <v>11</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="16" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="11" t="s">
@@ -1031,11 +1030,11 @@
       <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="25"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="9">
         <v>12</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="16" t="s">
         <v>14</v>
       </c>
       <c r="D20" s="11" t="s">
@@ -1055,11 +1054,11 @@
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="25"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="9">
         <v>13</v>
       </c>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="16" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="11" t="s">
@@ -1081,30 +1080,32 @@
       <c r="J21" s="11"/>
     </row>
     <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="26"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="13">
         <v>14</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="15" t="s">
+      <c r="D22" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
+      <c r="H22" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="J22" s="14"/>
     </row>
     <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
@@ -1210,15 +1211,15 @@
       <c r="B8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
     </row>
     <row r="9" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="1">

</xml_diff>

<commit_message>
Update Normalizacion de tablas.xlsx
</commit_message>
<xml_diff>
--- a/Normalizacion de tablas.xlsx
+++ b/Normalizacion de tablas.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778C3230-4A9D-45C6-B946-1321D8DD339F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -239,7 +240,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -410,6 +411,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -428,8 +431,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,6 +525,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -558,6 +577,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -733,12 +769,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A2:P30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="N28" sqref="A28:N32"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +795,7 @@
   <sheetData>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="27" t="s">
         <v>58</v>
       </c>
       <c r="C3" s="19" t="s">
@@ -806,13 +842,13 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="A4" s="27"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
+      <c r="A5" s="27"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="27"/>
     </row>
     <row r="8" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
@@ -820,21 +856,21 @@
       <c r="C8" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
     </row>
     <row r="9" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="24" t="s">
         <v>57</v>
       </c>
       <c r="B9" s="14">
@@ -858,7 +894,7 @@
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="9">
         <v>2</v>
       </c>
@@ -880,7 +916,7 @@
       <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="23"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="9">
         <v>3</v>
       </c>
@@ -919,7 +955,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="9">
         <v>4</v>
       </c>
@@ -941,7 +977,7 @@
       <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="9">
         <v>5</v>
       </c>
@@ -963,7 +999,7 @@
       <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="9">
         <v>6</v>
       </c>
@@ -985,7 +1021,7 @@
       <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="9">
         <v>7</v>
       </c>
@@ -1005,7 +1041,7 @@
       <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="9">
         <v>8</v>
       </c>
@@ -1027,7 +1063,7 @@
       <c r="J16" s="10"/>
     </row>
     <row r="17" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="9">
         <v>9</v>
       </c>
@@ -1049,7 +1085,7 @@
       <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="9">
         <v>10</v>
       </c>
@@ -1073,7 +1109,7 @@
       <c r="J18" s="10"/>
     </row>
     <row r="19" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="9">
         <v>11</v>
       </c>
@@ -1095,7 +1131,7 @@
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="23"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="9">
         <v>12</v>
       </c>
@@ -1119,7 +1155,7 @@
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="9">
         <v>13</v>
       </c>
@@ -1145,7 +1181,7 @@
       <c r="J21" s="10"/>
     </row>
     <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="24"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="12">
         <v>14</v>
       </c>
@@ -1189,12 +1225,13 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
+      <c r="F25" s="30"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B29" s="28">
+      <c r="B29" s="22">
         <v>3</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="22" t="s">
         <v>37</v>
       </c>
       <c r="D29" t="s">
@@ -1241,7 +1278,7 @@
       <c r="G30" t="s">
         <v>67</v>
       </c>
-      <c r="H30" s="29">
+      <c r="H30" s="23">
         <v>32111</v>
       </c>
       <c r="I30" t="s">
@@ -1272,7 +1309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A4:O24"/>
   <sheetViews>
@@ -1346,15 +1383,15 @@
       <c r="B8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
     </row>
     <row r="9" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="1">

</xml_diff>